<commit_message>
Fixed the clicking of cancel>> "No" click button crash.  Added more stability to code. Enable backing out of initializatio process then getting a prompt before closing out. Only the selection of no works
</commit_message>
<xml_diff>
--- a/BugsToBeFixedScreenSavings.xlsx
+++ b/BugsToBeFixedScreenSavings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Fix dumy tokens </t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Write Php script to clear entry for ease</t>
+  </si>
+  <si>
+    <t>write php script to reset everything with app</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B14"/>
+  <dimension ref="B3:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,6 +451,11 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed  Finish Will need UI enhancements
</commit_message>
<xml_diff>
--- a/BugsToBeFixedScreenSavings.xlsx
+++ b/BugsToBeFixedScreenSavings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Fix dumy tokens </t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>write php script to reset everything with app</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B15"/>
+  <dimension ref="B3:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,67 +394,70 @@
     <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Current update loads cache on app load up and fixed initialization sequence issues.
</commit_message>
<xml_diff>
--- a/BugsToBeFixedScreenSavings.xlsx
+++ b/BugsToBeFixedScreenSavings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t xml:space="preserve">Fix dumy tokens </t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>fix Configuration menu</t>
+  </si>
+  <si>
+    <t>fix background notification bug caused by launcing application w/o internet and then logging in with internet</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D18"/>
+  <dimension ref="B3:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +442,9 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
       <c r="D7">
         <v>3</v>
       </c>
@@ -458,6 +464,9 @@
       <c r="B9" t="s">
         <v>4</v>
       </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
       <c r="D9">
         <v>4</v>
       </c>
@@ -526,6 +535,11 @@
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates fixes most synchronization issues and works with rapid start
</commit_message>
<xml_diff>
--- a/BugsToBeFixedScreenSavings.xlsx
+++ b/BugsToBeFixedScreenSavings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t xml:space="preserve">Fix dumy tokens </t>
   </si>
@@ -78,6 +78,51 @@
   </si>
   <si>
     <t>fix background notification bug caused by launcing application w/o internet and then logging in with internet</t>
+  </si>
+  <si>
+    <t>Remove entry in cache when service is unregistered.</t>
+  </si>
+  <si>
+    <t>Remove entry in UI when service is unregistered.</t>
+  </si>
+  <si>
+    <t>Order Element in UI based on Time independent of the service</t>
+  </si>
+  <si>
+    <t>setup cron job for PHP</t>
+  </si>
+  <si>
+    <t>Investigate how you can have intelligent caching on server</t>
+  </si>
+  <si>
+    <t>See if you can use gmail atom to retrieve email</t>
+  </si>
+  <si>
+    <t>Setup groupon for cache and make appropriate calls</t>
+  </si>
+  <si>
+    <t>Remove entry in database cache when service is unregistered.</t>
+  </si>
+  <si>
+    <t>Fix look of setup when I right click while on settings menu.</t>
+  </si>
+  <si>
+    <t>Add other service like instagram yahoo and other deals</t>
+  </si>
+  <si>
+    <t>fix getData function to have option for saving refreshed data to dbase</t>
+  </si>
+  <si>
+    <t>Provide ability to reply to tweets, facebookpost and email</t>
+  </si>
+  <si>
+    <t>Fix weird twitter bug of double login failure crash</t>
+  </si>
+  <si>
+    <t>Provide option for removing/adding image from cached rapid start storage</t>
+  </si>
+  <si>
+    <t>Add Weather widget</t>
   </si>
 </sst>
 </file>
@@ -395,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D19"/>
+  <dimension ref="B3:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,72 +461,78 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
         <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -489,7 +540,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -497,7 +548,7 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -505,40 +556,184 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Latest update fixes ui elements
Adds live functional weather information
</commit_message>
<xml_diff>
--- a/BugsToBeFixedScreenSavings.xlsx
+++ b/BugsToBeFixedScreenSavings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t xml:space="preserve">Fix dumy tokens </t>
   </si>
@@ -443,7 +443,7 @@
   <dimension ref="B3:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,9 +722,6 @@
       <c r="B35" t="s">
         <v>30</v>
       </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
       <c r="D35">
         <v>16</v>
       </c>

</xml_diff>